<commit_message>
Support Predictions for Collaborative Recommender
</commit_message>
<xml_diff>
--- a/ProjectLog.xlsx
+++ b/ProjectLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\animeRecommendationSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4362FB-CBF3-461B-B134-B1A947BDB481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E522A-7F35-4DF4-B411-D15E1F5E3245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>Date Finished</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Support cross validation for the CBF model</t>
+  </si>
+  <si>
+    <t>Compare different algorithms e.g. KNNWithMeans, KNNWithZScore etc.</t>
+  </si>
+  <si>
+    <t>Perform a GridSearch to hypertune the algorithm parameters</t>
   </si>
 </sst>
 </file>
@@ -304,7 +310,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -319,7 +325,6 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -330,6 +335,69 @@
   <dxfs count="21">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -348,6 +416,91 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -422,59 +575,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -493,17 +593,12 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -534,110 +629,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -671,54 +676,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B176215D-3E25-465E-8734-F770A2BFE3F2}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B176215D-3E25-465E-8734-F770A2BFE3F2}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:C7" xr:uid="{B176215D-3E25-465E-8734-F770A2BFE3F2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DFDAABA4-5AB9-48CB-AD77-74292D9825B2}" name="Overall Task" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C07F7294-7A13-4F13-AAC7-AC98E74B30A3}" name="Priority" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{FD6E8A6E-BBFA-480B-A476-D504B27D722A}" name="Data Finished" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{DFDAABA4-5AB9-48CB-AD77-74292D9825B2}" name="Overall Task" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C07F7294-7A13-4F13-AAC7-AC98E74B30A3}" name="Priority" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{FD6E8A6E-BBFA-480B-A476-D504B27D722A}" name="Data Finished" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{32B3F3BC-3213-4C32-AA1A-ED29D5C27049}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{32B3F3BC-3213-4C32-AA1A-ED29D5C27049}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:D6" xr:uid="{32B3F3BC-3213-4C32-AA1A-ED29D5C27049}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C6A5278-DB72-42E0-A0F9-AA634A2D59A4}" name="Sub-Task" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{6EB5F5B7-4985-43EC-A269-119ED4ED1161}" name="Priority" dataDxfId="3" dataCellStyle="Bad"/>
-    <tableColumn id="3" xr3:uid="{1ED58AB5-59A7-47BE-B508-A9EC0B64F4AD}" name="Finished?" dataDxfId="2" dataCellStyle="Good"/>
-    <tableColumn id="4" xr3:uid="{0EEA310E-C110-453D-BE5A-690D8D2AF76D}" name="Date Finished" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8C6A5278-DB72-42E0-A0F9-AA634A2D59A4}" name="Sub-Task" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{6EB5F5B7-4985-43EC-A269-119ED4ED1161}" name="Priority" dataDxfId="13" dataCellStyle="Bad"/>
+    <tableColumn id="3" xr3:uid="{1ED58AB5-59A7-47BE-B508-A9EC0B64F4AD}" name="Finished?" dataDxfId="12" dataCellStyle="Good"/>
+    <tableColumn id="4" xr3:uid="{0EEA310E-C110-453D-BE5A-690D8D2AF76D}" name="Date Finished" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="20" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:D14" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
     <sortCondition descending="1" ref="D1:D13"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB039294-D058-4731-B655-F5AC2D298968}" name="Sub-Task" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{70DD6EBE-8696-483F-9161-21B8F4F67AED}" name="Priority" dataDxfId="18" dataCellStyle="Neutral"/>
-    <tableColumn id="3" xr3:uid="{EF59A110-B41A-4B19-8713-54C02158BE15}" name="Completed?" dataDxfId="17" dataCellStyle="Good"/>
-    <tableColumn id="4" xr3:uid="{0BDA4045-6557-4C5D-89AC-BE67E3FD7FA3}" name="Completion Date" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{DB039294-D058-4731-B655-F5AC2D298968}" name="Sub-Task" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{70DD6EBE-8696-483F-9161-21B8F4F67AED}" name="Priority" dataDxfId="7" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{EF59A110-B41A-4B19-8713-54C02158BE15}" name="Completed?" dataDxfId="6" dataCellStyle="Good"/>
+    <tableColumn id="4" xr3:uid="{0BDA4045-6557-4C5D-89AC-BE67E3FD7FA3}" name="Completion Date" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}" name="Table2" displayName="Table2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:D8" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}" name="Table2" displayName="Table2" ref="A1:D10" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D10" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4474FE88-BF57-400E-B557-D9F7792BD945}" name="Sub-Task" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{90D4ABA7-9778-4978-8446-83BD66FD4CC5}" name="Priority" dataDxfId="12" dataCellStyle="Bad"/>
-    <tableColumn id="3" xr3:uid="{FA391E9E-6976-444D-9478-02E2D7D60B53}" name="Finished?" dataDxfId="11" dataCellStyle="Bad"/>
-    <tableColumn id="4" xr3:uid="{232FD672-1458-4341-94CD-2FC92FFB01F5}" name="Date Finished" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{4474FE88-BF57-400E-B557-D9F7792BD945}" name="Sub-Task" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{90D4ABA7-9778-4978-8446-83BD66FD4CC5}" name="Priority" dataDxfId="2" dataCellStyle="Bad"/>
+    <tableColumn id="3" xr3:uid="{FA391E9E-6976-444D-9478-02E2D7D60B53}" name="Finished?" dataDxfId="1" dataCellStyle="Bad"/>
+    <tableColumn id="4" xr3:uid="{232FD672-1458-4341-94CD-2FC92FFB01F5}" name="Date Finished" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1023,18 +1028,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564A22F4-1C3D-4A06-A6DE-506EEA3469F5}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1045,7 +1050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
@@ -1056,7 +1061,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -1065,7 +1070,7 @@
       </c>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1074,7 +1079,7 @@
       </c>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1088,7 @@
       </c>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -1092,7 +1097,7 @@
       </c>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -1117,15 +1122,15 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1158,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1167,7 +1172,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1186,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1195,7 +1200,7 @@
         <v>45199</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1226,15 +1231,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1248,7 +1253,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
@@ -1262,7 +1267,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
@@ -1276,7 +1281,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1304,7 +1309,7 @@
         <v>45306</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1318,7 +1323,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1332,7 +1337,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1346,7 +1351,7 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -1360,7 +1365,7 @@
         <v>45243</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -1374,7 +1379,7 @@
         <v>45243</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -1386,7 +1391,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1398,7 +1403,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
@@ -1410,7 +1415,7 @@
       </c>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>45</v>
       </c>
@@ -1432,21 +1437,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB981B5-0229-4450-9452-8FF3F7ACB3A8}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1460,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -1474,7 +1479,7 @@
         <v>45313</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
@@ -1488,7 +1493,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>44</v>
       </c>
@@ -1500,7 +1505,7 @@
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
@@ -1512,41 +1517,69 @@
       </c>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9">
+        <v>45319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9">
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1564,12 +1597,12 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1596,12 +1629,12 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Support SVD for the Collaborative Filtering
</commit_message>
<xml_diff>
--- a/ProjectLog.xlsx
+++ b/ProjectLog.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\animeRecommendationSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A8436F-DABD-4B62-8645-FC45AA7707AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C480D75-0620-4994-B768-AD2CB17F594A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
     <sheet name="Data Collection" sheetId="1" r:id="rId2"/>
     <sheet name="Content-Based Filtering" sheetId="2" r:id="rId3"/>
     <sheet name="Collaborative Filtering" sheetId="3" r:id="rId4"/>
-    <sheet name="New Users Evaluation" sheetId="6" r:id="rId5"/>
+    <sheet name="Multiple Datasets Evaluation" sheetId="6" r:id="rId5"/>
     <sheet name="Web Interface" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Date Finished</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Switch the CBF recommender to support multiple distance metrics e.g. cosine distance, euclidean distance</t>
   </si>
   <si>
-    <t>Support RMSE for evaluating the CBF recommender</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Very Low</t>
   </si>
   <si>
-    <t>Evaluate the systems for new users</t>
-  </si>
-  <si>
     <t>Change evaluation metric to work per user (i.e. for the predictions made for that user)</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Improve the vectorisation of  anime</t>
   </si>
   <si>
-    <t>Add other distance metrics to compare with</t>
-  </si>
-  <si>
     <t>Completed?</t>
   </si>
   <si>
@@ -188,13 +179,35 @@
     <t>Support cross validation for the CBF model</t>
   </si>
   <si>
-    <t>Compare different algorithms e.g. KNNWithMeans, KNNWithZScore etc.</t>
-  </si>
-  <si>
-    <t>Perform a GridSearch to hypertune the algorithm parameters</t>
-  </si>
-  <si>
-    <t>Make the recommend user function predict the rating for its neighbour's items</t>
+    <t>Compare different algorithms e.g. SVD, SVD++ etc.</t>
+  </si>
+  <si>
+    <t>Switch to use SVD</t>
+  </si>
+  <si>
+    <t>Perform a GridSearch to hypertune the algorithm parameters for the final model</t>
+  </si>
+  <si>
+    <t>Fix any remaining issues with the recommender</t>
+  </si>
+  <si>
+    <t>Evaluate the recommenders using multiple datasets</t>
+  </si>
+  <si>
+    <t>Rename the existing user ratings dataset
+as the standard set</t>
+  </si>
+  <si>
+    <t>Add the new users dataset</t>
+  </si>
+  <si>
+    <t>Evaluate each recommender on the new users dataset</t>
+  </si>
+  <si>
+    <t>Create graphs comparing the performance on both datasets</t>
+  </si>
+  <si>
+    <t>Remove watching and dropped shows from both datasets</t>
   </si>
 </sst>
 </file>
@@ -335,7 +348,90 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -679,54 +775,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B176215D-3E25-465E-8734-F770A2BFE3F2}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B176215D-3E25-465E-8734-F770A2BFE3F2}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:C7" xr:uid="{B176215D-3E25-465E-8734-F770A2BFE3F2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DFDAABA4-5AB9-48CB-AD77-74292D9825B2}" name="Overall Task" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{C07F7294-7A13-4F13-AAC7-AC98E74B30A3}" name="Priority" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{FD6E8A6E-BBFA-480B-A476-D504B27D722A}" name="Data Finished" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{DFDAABA4-5AB9-48CB-AD77-74292D9825B2}" name="Overall Task" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{C07F7294-7A13-4F13-AAC7-AC98E74B30A3}" name="Priority" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{FD6E8A6E-BBFA-480B-A476-D504B27D722A}" name="Data Finished" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{32B3F3BC-3213-4C32-AA1A-ED29D5C27049}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{32B3F3BC-3213-4C32-AA1A-ED29D5C27049}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A1:D6" xr:uid="{32B3F3BC-3213-4C32-AA1A-ED29D5C27049}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C6A5278-DB72-42E0-A0F9-AA634A2D59A4}" name="Sub-Task" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{6EB5F5B7-4985-43EC-A269-119ED4ED1161}" name="Priority" dataDxfId="13" dataCellStyle="Bad"/>
-    <tableColumn id="3" xr3:uid="{1ED58AB5-59A7-47BE-B508-A9EC0B64F4AD}" name="Finished?" dataDxfId="12" dataCellStyle="Good"/>
-    <tableColumn id="4" xr3:uid="{0EEA310E-C110-453D-BE5A-690D8D2AF76D}" name="Date Finished" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{8C6A5278-DB72-42E0-A0F9-AA634A2D59A4}" name="Sub-Task" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{6EB5F5B7-4985-43EC-A269-119ED4ED1161}" name="Priority" dataDxfId="19" dataCellStyle="Bad"/>
+    <tableColumn id="3" xr3:uid="{1ED58AB5-59A7-47BE-B508-A9EC0B64F4AD}" name="Finished?" dataDxfId="18" dataCellStyle="Good"/>
+    <tableColumn id="4" xr3:uid="{0EEA310E-C110-453D-BE5A-690D8D2AF76D}" name="Date Finished" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:D14" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
-    <sortCondition descending="1" ref="D1:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:D13" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
+    <sortCondition descending="1" ref="D1:D11"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB039294-D058-4731-B655-F5AC2D298968}" name="Sub-Task" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{70DD6EBE-8696-483F-9161-21B8F4F67AED}" name="Priority" dataDxfId="7" dataCellStyle="Neutral"/>
-    <tableColumn id="3" xr3:uid="{EF59A110-B41A-4B19-8713-54C02158BE15}" name="Completed?" dataDxfId="6" dataCellStyle="Good"/>
-    <tableColumn id="4" xr3:uid="{0BDA4045-6557-4C5D-89AC-BE67E3FD7FA3}" name="Completion Date" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{DB039294-D058-4731-B655-F5AC2D298968}" name="Sub-Task" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{70DD6EBE-8696-483F-9161-21B8F4F67AED}" name="Priority" dataDxfId="13" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{EF59A110-B41A-4B19-8713-54C02158BE15}" name="Completed?" dataDxfId="12" dataCellStyle="Good"/>
+    <tableColumn id="4" xr3:uid="{0BDA4045-6557-4C5D-89AC-BE67E3FD7FA3}" name="Completion Date" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}" name="Table2" displayName="Table2" ref="A1:D11" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}" name="Table2" displayName="Table2" ref="A1:D11" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:D11" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4474FE88-BF57-400E-B557-D9F7792BD945}" name="Sub-Task" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{90D4ABA7-9778-4978-8446-83BD66FD4CC5}" name="Priority" dataDxfId="2" dataCellStyle="Bad"/>
-    <tableColumn id="3" xr3:uid="{FA391E9E-6976-444D-9478-02E2D7D60B53}" name="Finished?" dataDxfId="1" dataCellStyle="Bad"/>
-    <tableColumn id="4" xr3:uid="{232FD672-1458-4341-94CD-2FC92FFB01F5}" name="Date Finished" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4474FE88-BF57-400E-B557-D9F7792BD945}" name="Sub-Task" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{90D4ABA7-9778-4978-8446-83BD66FD4CC5}" name="Priority" dataDxfId="8" dataCellStyle="Bad"/>
+    <tableColumn id="3" xr3:uid="{FA391E9E-6976-444D-9478-02E2D7D60B53}" name="Finished?" dataDxfId="7" dataCellStyle="Bad"/>
+    <tableColumn id="4" xr3:uid="{232FD672-1458-4341-94CD-2FC92FFB01F5}" name="Date Finished" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5987DAE0-31B3-417C-A459-2199DA8AF84A}" name="Table5" displayName="Table5" ref="A1:D6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
+  <autoFilter ref="A1:D6" xr:uid="{5987DAE0-31B3-417C-A459-2199DA8AF84A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{006AF1B9-7134-4425-8E3D-7EE31C14165A}" name="Sub-Task" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{FAAC91C6-B4C3-4D08-9E2E-359AA41B8DDF}" name="Priority" dataDxfId="3" dataCellStyle="Bad"/>
+    <tableColumn id="3" xr3:uid="{91A0D836-1D9F-444C-BCEB-A007F894E443}" name="Finished?" dataDxfId="2" dataCellStyle="Bad"/>
+    <tableColumn id="4" xr3:uid="{D504C7DC-E345-40D0-B6DB-9901B58B2D63}" name="Date Finished" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1032,7 +1141,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,21 +1153,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="9">
         <v>45222</v>
@@ -1066,7 +1175,7 @@
     </row>
     <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -1075,7 +1184,7 @@
     </row>
     <row r="4" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>9</v>
@@ -1084,16 +1193,16 @@
     </row>
     <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>9</v>
@@ -1102,10 +1211,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="11"/>
     </row>
@@ -1135,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1228,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A34CCC9-24A7-4EB0-B684-B237532D90B3}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,21 +1353,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>9</v>
@@ -1272,7 +1381,7 @@
     </row>
     <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>9</v>
@@ -1286,10 +1395,10 @@
     </row>
     <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>4</v>
@@ -1300,7 +1409,7 @@
     </row>
     <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>9</v>
@@ -1314,7 +1423,7 @@
     </row>
     <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>9</v>
@@ -1328,7 +1437,7 @@
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>9</v>
@@ -1382,53 +1491,41 @@
         <v>45243</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="9"/>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1442,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB981B5-0229-4450-9452-8FF3F7ACB3A8}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1553,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1470,7 +1567,7 @@
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -1484,7 +1581,7 @@
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
@@ -1498,31 +1595,31 @@
     </row>
     <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
@@ -1536,7 +1633,7 @@
     </row>
     <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -1548,51 +1645,53 @@
         <v>45320</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9">
+        <v>45321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="11"/>
     </row>
@@ -1606,33 +1705,99 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8604CB-AB2D-4350-BE93-5DBC8A579841}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1651,7 +1816,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Added Hit Rate Evaluation
</commit_message>
<xml_diff>
--- a/ProjectLog.xlsx
+++ b/ProjectLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\animeRecommendationSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66346B9E-541F-45A7-B68B-CB916D12DFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C175C98-8B63-4878-8D07-3391B29FF8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
   <si>
     <t>Date Finished</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Remove the distance column from the recommendations table</t>
+  </si>
+  <si>
+    <t>Fix Collaborative Recommenders so they show their recommendations results</t>
   </si>
 </sst>
 </file>
@@ -946,13 +949,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}" name="Table6" displayName="Table6" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
-  <autoFilter ref="A1:D9" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}" name="Table6" displayName="Table6" ref="A1:D10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D10" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{26605586-3F46-4C27-B53E-0B2CFB20FB73}" name="Sub-Task" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A11E8E77-60BF-4C5D-BC84-EBF734E41015}" name="Priority" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{276FEEC7-4300-4EBF-86F1-C7B528D2A6C8}" name="Finished?" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{BB8D4FF8-EDD1-4E2F-A53F-A255187C8C12}" name="Date Finished" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{26605586-3F46-4C27-B53E-0B2CFB20FB73}" name="Sub-Task" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A11E8E77-60BF-4C5D-BC84-EBF734E41015}" name="Priority" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{276FEEC7-4300-4EBF-86F1-C7B528D2A6C8}" name="Finished?" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BB8D4FF8-EDD1-4E2F-A53F-A255187C8C12}" name="Date Finished" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1946,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B61A5E7-19A9-4FD2-833D-41A2C1AAEB17}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,21 +2059,21 @@
         <v>45357</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -2079,6 +2082,18 @@
         <v>14</v>
       </c>
       <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved the Streamlit App
</commit_message>
<xml_diff>
--- a/ProjectLog.xlsx
+++ b/ProjectLog.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\animeRecommendationSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C175C98-8B63-4878-8D07-3391B29FF8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1210926B-9433-4F7B-B5D7-89D4AB2ED7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B032F3D-D160-4714-92A2-1D8BD243C1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
     <sheet name="Data Collection" sheetId="1" r:id="rId2"/>
     <sheet name="Content-Based Filtering" sheetId="2" r:id="rId3"/>
     <sheet name="Collaborative Filtering" sheetId="3" r:id="rId4"/>
-    <sheet name="Multiple Datasets Evaluation" sheetId="6" r:id="rId5"/>
-    <sheet name="Web Interface" sheetId="5" r:id="rId6"/>
+    <sheet name="Hybrid System" sheetId="7" r:id="rId5"/>
+    <sheet name="Multiple Datasets Evaluation" sheetId="6" r:id="rId6"/>
+    <sheet name="Web Interface" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>Date Finished</t>
   </si>
@@ -145,9 +146,6 @@
     <t>Update the test recommendations function to work with the new evaluation method</t>
   </si>
   <si>
-    <t>Improve the vectorisation of  anime</t>
-  </si>
-  <si>
     <t>Completed?</t>
   </si>
   <si>
@@ -170,15 +168,9 @@
     <t>Create a graph that looks like the CBF evaluation graph</t>
   </si>
   <si>
-    <t>Normalise the user ratings per user</t>
-  </si>
-  <si>
     <t>Remove shows that have not been finished, or have been dropped.</t>
   </si>
   <si>
-    <t>Support cross validation for the CBF model</t>
-  </si>
-  <si>
     <t>Compare different algorithms e.g. SVD, SVD++ etc.</t>
   </si>
   <si>
@@ -188,14 +180,7 @@
     <t>Perform a GridSearch to hypertune the algorithm parameters for the final model</t>
   </si>
   <si>
-    <t>Fix any remaining issues with the recommender</t>
-  </si>
-  <si>
     <t>Evaluate the recommenders using multiple datasets</t>
-  </si>
-  <si>
-    <t>Rename the existing user ratings dataset
-as the standard set</t>
   </si>
   <si>
     <t>Add the new users dataset</t>
@@ -233,13 +218,13 @@
     <t>Add a second page showing the evaluation results</t>
   </si>
   <si>
-    <t>Allow selectable evaluation options i.e. All Recommender, CBF Recommender etc.</t>
-  </si>
-  <si>
     <t>Remove the distance column from the recommendations table</t>
   </si>
   <si>
     <t>Fix Collaborative Recommenders so they show their recommendations results</t>
+  </si>
+  <si>
+    <t>Fix any remaining bugs</t>
   </si>
 </sst>
 </file>
@@ -907,10 +892,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:D13" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
-    <sortCondition descending="1" ref="D1:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:D11" xr:uid="{55C6B186-3084-4BE6-A79A-AA3CB9B18C52}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">
+    <sortCondition descending="1" ref="D1:D10"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{DB039294-D058-4731-B655-F5AC2D298968}" name="Sub-Task" dataDxfId="20"/>
@@ -923,8 +908,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}" name="Table2" displayName="Table2" ref="A1:D11" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:D11" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}" name="Table2" displayName="Table2" ref="A1:D10" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:D10" xr:uid="{759D4793-D161-4BD4-81FA-FF592A94C73B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4474FE88-BF57-400E-B557-D9F7792BD945}" name="Sub-Task" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{90D4ABA7-9778-4978-8446-83BD66FD4CC5}" name="Priority" dataDxfId="14" dataCellStyle="Bad"/>
@@ -936,8 +921,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5987DAE0-31B3-417C-A459-2199DA8AF84A}" name="Table5" displayName="Table5" ref="A1:D7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D7" xr:uid="{5987DAE0-31B3-417C-A459-2199DA8AF84A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5987DAE0-31B3-417C-A459-2199DA8AF84A}" name="Table5" displayName="Table5" ref="A1:D6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D6" xr:uid="{5987DAE0-31B3-417C-A459-2199DA8AF84A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{006AF1B9-7134-4425-8E3D-7EE31C14165A}" name="Sub-Task" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{FAAC91C6-B4C3-4D08-9E2E-359AA41B8DDF}" name="Priority" dataDxfId="8" dataCellStyle="Bad"/>
@@ -949,8 +934,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}" name="Table6" displayName="Table6" ref="A1:D10" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D10" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}" name="Table6" displayName="Table6" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D9" xr:uid="{04659E97-F0C7-416A-980A-020311B46609}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{26605586-3F46-4C27-B53E-0B2CFB20FB73}" name="Sub-Task" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{A11E8E77-60BF-4C5D-BC84-EBF734E41015}" name="Priority" dataDxfId="2"/>
@@ -1260,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{564A22F4-1C3D-4A06-A6DE-506EEA3469F5}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1285,9 @@
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="8">
+        <v>45366</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1322,12 +1309,14 @@
     </row>
     <row r="6" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="8">
+        <v>45366</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1336,7 +1325,9 @@
       <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="8">
+        <v>45367</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1351,7 +1342,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A34CCC9-24A7-4EB0-B684-B237532D90B3}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,10 +1470,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
@@ -1611,41 +1602,19 @@
         <v>45243</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8"/>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>45366</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1657,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB981B5-0229-4450-9452-8FF3F7ACB3A8}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1656,7 @@
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -1701,7 +1670,7 @@
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -1715,7 +1684,7 @@
     </row>
     <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
@@ -1729,61 +1698,63 @@
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>45319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>45319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>45321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="8">
-        <v>45320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="8">
-        <v>45321</v>
+        <v>45332</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -1791,35 +1762,21 @@
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="11">
         <v>45332</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="11">
-        <v>45332</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1830,11 +1787,43 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8604CB-AB2D-4350-BE93-5DBC8A579841}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A000F2-7B36-49F4-A447-AD557E7FBC45}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8604CB-AB2D-4350-BE93-5DBC8A579841}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,21 +1848,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8">
+        <v>45339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -1882,38 +1873,40 @@
         <v>4</v>
       </c>
       <c r="D3" s="8">
+        <v>45341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
         <v>45339</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8">
-        <v>45341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -1922,20 +1915,6 @@
         <v>4</v>
       </c>
       <c r="D6" s="8">
-        <v>45339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="8">
         <v>45339</v>
       </c>
     </row>
@@ -1947,12 +1926,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B61A5E7-19A9-4FD2-833D-41A2C1AAEB17}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +1958,7 @@
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -1993,7 +1972,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -2005,7 +1984,7 @@
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>9</v>
@@ -2019,7 +1998,7 @@
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -2033,7 +2012,7 @@
     </row>
     <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>9</v>
@@ -2047,7 +2026,7 @@
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -2061,39 +2040,31 @@
     </row>
     <row r="8" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>45367</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="8"/>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>45367</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>